<commit_message>
Update Excel with new data
</commit_message>
<xml_diff>
--- a/New_home.xlsx
+++ b/New_home.xlsx
@@ -9096,7 +9096,11 @@
       </c>
     </row>
     <row r="50">
-      <c r="B50" s="4" t="n"/>
+      <c r="B50" s="4" t="inlineStr">
+        <is>
+          <t>ESTO ES UNA PRUEBA</t>
+        </is>
+      </c>
       <c r="C50" s="10" t="n"/>
       <c r="D50" s="9" t="n"/>
       <c r="E50" s="9" t="n"/>
@@ -33055,8 +33059,8 @@
   <mergeCells count="10">
     <mergeCell ref="C2:E3"/>
     <mergeCell ref="AJ3:AK3"/>
+    <mergeCell ref="AH2:AI2"/>
     <mergeCell ref="AH3:AI3"/>
-    <mergeCell ref="AH2:AI2"/>
     <mergeCell ref="F2:G3"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="AJ2:AK2"/>

</xml_diff>